<commit_message>
Forgot to save it...
</commit_message>
<xml_diff>
--- a/Game notes.xlsx
+++ b/Game notes.xlsx
@@ -16,6 +16,23 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Number</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -331,12 +348,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="4" max="4" width="112.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added death sound note
</commit_message>
<xml_diff>
--- a/Game notes.xlsx
+++ b/Game notes.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="21">
   <si>
     <t>Type</t>
   </si>
@@ -76,6 +76,12 @@
   </si>
   <si>
     <t>Plays when near windmill</t>
+  </si>
+  <si>
+    <t>Death sound</t>
+  </si>
+  <si>
+    <t>Plays when player runs out of health</t>
   </si>
 </sst>
 </file>
@@ -393,10 +399,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -517,6 +523,20 @@
         <v>18</v>
       </c>
     </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" t="s">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>